<commit_message>
new grouped racial category
</commit_message>
<xml_diff>
--- a/Output.data/dictionary.xlsx
+++ b/Output.data/dictionary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,173 +409,187 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ethnic.appearance</t>
+          <t>Racialised</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ethnic.Appearance.original</t>
+          <t>Ethnic.appearance</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Found</t>
+          <t>Ethnic.Appearance.original</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Search.type - Drugs</t>
+          <t>Ethnic.appearance.abridged</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Search.type - Weapons</t>
+          <t>Found</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Search.type - Firearms</t>
+          <t>Search.type - Drugs</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Search.type - Graffiti</t>
+          <t>Search.type - Weapons</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Search.type - Volatile.sub.U18</t>
+          <t>Search.type - Firearms</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Search.type - Volatile.sub.adult</t>
+          <t>Search.type - Graffiti</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Indigenous.Status</t>
+          <t>Search.type - Volatile.sub.U18</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Search.type - Volatile.sub.adult</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Indigenous.Status</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Complexion</t>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hair.Colour</t>
+          <t>Age</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hair.Style</t>
+          <t>Complexion</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Reporting.Station.Description</t>
+          <t>Hair.Colour</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Unit.type</t>
+          <t>Hair.Style</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Rank.of.Member</t>
+          <t>Reporting.Station.Description</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Region</t>
+          <t>Unit.type</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Division</t>
+          <t>Rank.of.Member</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Police.Service.Area</t>
+          <t>Region</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Area.type</t>
+          <t>Division</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Local.Government.Area</t>
+          <t>Police.Service.Area</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Locality</t>
+          <t>Area.type</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
+        <is>
+          <t>Local.Government.Area</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Locality</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Postcode</t>
         </is>

</xml_diff>